<commit_message>
remove completed tasks from list
</commit_message>
<xml_diff>
--- a/project_mgmt.xlsx
+++ b/project_mgmt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t xml:space="preserve">WHAT</t>
   </si>
@@ -78,91 +78,46 @@
     <t xml:space="preserve">Add ages and genders to injury dataset @rahulatiitd to work on this; @robj411 suggested using only the cases with age and gender and account for other cases using reporting level as a parameter</t>
   </si>
   <si>
-    <t xml:space="preserve">RG, RJ</t>
-  </si>
-  <si>
     <t xml:space="preserve">Use without covariates</t>
   </si>
   <si>
-    <t xml:space="preserve">PA summary tables</t>
+    <t xml:space="preserve">Sort out travel data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distribution for BUS_WALK_TIME, if walk to bus is added. @usr110 and @leandromtg to look at this distribution from reported numbers in Sao Paulo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA, LG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use lnorm(1.6, 0.23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@rahulatiitd also to estimate this for Delhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distribution for BACKGROUND_PA_SCALAR (amount to scale non-zero, non-travel PA)</t>
   </si>
   <si>
     <t xml:space="preserve">All</t>
   </si>
   <si>
-    <t xml:space="preserve">LG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP summary tables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Injuries summary tables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP+PA health summary tables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Injury health summary tables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sort out travel data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add stages to trips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ac. and Ban.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Happens in situ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change ‘other’ to ‘motorcycle’</t>
+    <t xml:space="preserve">JW, LG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use lnorm(0, 0.18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number for BACKGROUND_PA_CONFIDENCE (how confident are you about the number of zeros in the PA survey on a scale of 0 to 1?)</t>
   </si>
   <si>
     <t xml:space="preserve">Accra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distribution for BUS_WALK_TIME, if walk to bus is added. @usr110 and @leandromtg to look at this distribution from reported numbers in Sao Paulo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AA, LG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use lnorm(1.6, 0.23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@rahulatiitd also to estimate this for Delhi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distribution for BACKGROUND_PA_SCALAR (amount to scale non-zero, non-travel PA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JW, LG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use lnorm(0, 0.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number for BACKGROUND_PA_CONFIDENCE (how confident are you about the number of zeros in the PA survey on a scale of 0 to 1?)</t>
   </si>
   <si>
     <t xml:space="preserve">number for BACKGROUND_PA_CONFIDENCE</t>
@@ -200,7 +155,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -245,12 +200,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -381,7 +330,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,38 +431,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -534,24 +451,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -632,10 +537,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -645,9 +550,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -780,7 +685,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F6" s="17" t="n">
         <v>43581</v>
@@ -789,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,241 +702,34 @@
         <v>7</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>43581</v>
+      </c>
+      <c r="G7" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="21" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G7" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="12" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G8" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="17" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G9" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="21" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G10" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
-        <v>11</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="12" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G11" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
-        <v>12</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="17" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G12" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="21" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G13" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
-        <v>14</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="12" t="n">
-        <v>43581</v>
-      </c>
-      <c r="G14" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="26" t="n">
-        <v>43588</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="n">
-        <v>16</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="30" t="n">
-        <v>43588</v>
-      </c>
-      <c r="G16" s="31" t="n">
-        <v>5</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1050,7 +748,7 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
@@ -1062,7 +760,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
@@ -1093,14 +791,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="9"/>
-      <c r="C2" s="33" t="s">
-        <v>37</v>
+      <c r="C2" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F2" s="12" t="n">
         <v>43581</v>
@@ -1109,7 +807,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,11 +815,11 @@
         <v>3</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="34" t="s">
-        <v>41</v>
+      <c r="C3" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>11</v>
@@ -1133,7 +831,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,21 +839,21 @@
         <v>4</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="35" t="s">
-        <v>42</v>
+      <c r="C4" s="27" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22" t="n">
         <v>5</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1163,20 +861,20 @@
         <v>5</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="36" t="s">
-        <v>45</v>
+      <c r="C5" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="37" t="n">
+      <c r="H5" s="29" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1185,20 +883,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="38" t="s">
-        <v>46</v>
+      <c r="C6" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="H6" s="39" t="n">
+      <c r="H6" s="30" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -1207,20 +905,20 @@
         <v>7</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="40" t="s">
-        <v>46</v>
+      <c r="C7" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="41" t="n">
+      <c r="H7" s="31" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -1229,20 +927,20 @@
         <v>8</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="42" t="s">
-        <v>46</v>
+      <c r="C8" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="37" t="n">
+      <c r="H8" s="29" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -1251,21 +949,21 @@
         <v>9</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="34" t="s">
-        <v>48</v>
+      <c r="C9" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,8 +971,8 @@
         <v>10</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="35" t="s">
-        <v>50</v>
+      <c r="C10" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>14</v>
@@ -1287,7 +985,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,8 +993,8 @@
         <v>11</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="36" t="s">
-        <v>52</v>
+      <c r="C11" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>14</v>
@@ -1309,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,14 +1015,14 @@
         <v>12</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="35" t="s">
-        <v>54</v>
+      <c r="C12" s="27" t="s">
+        <v>39</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="22" t="n">

</xml_diff>